<commit_message>
datos generados de distancias
</commit_message>
<xml_diff>
--- a/data/Dades_Municipis.xlsx
+++ b/data/Dades_Municipis.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1603" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1603" uniqueCount="682">
   <si>
     <t xml:space="preserve">Lot 2</t>
   </si>
@@ -1177,9 +1177,6 @@
   </si>
   <si>
     <t xml:space="preserve">Llacuna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conca Barb.</t>
   </si>
   <si>
     <t xml:space="preserve">Conesa</t>
@@ -1769,9 +1766,6 @@
     <t xml:space="preserve">Collbató</t>
   </si>
   <si>
-    <t xml:space="preserve">Vallès Occ.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Rellinars</t>
   </si>
   <si>
@@ -1779,9 +1773,6 @@
   </si>
   <si>
     <t xml:space="preserve">Òrrius</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vallès Ori.</t>
   </si>
   <si>
     <t xml:space="preserve">Santa Maria de Martorelles</t>
@@ -6930,7 +6921,7 @@
   <dimension ref="A1:U325"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C51" activeCellId="0" sqref="C51"/>
+      <selection pane="topLeft" activeCell="C51" activeCellId="1" sqref="C22:C25 C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14571,8 +14562,8 @@
   </sheetPr>
   <dimension ref="A1:G104"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A83" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F45" activeCellId="0" sqref="F45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="C22:C25 C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15092,7 +15083,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>2</v>
       </c>
@@ -15100,13 +15091,13 @@
         <v>1</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>382</v>
+        <v>38</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>43046</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>109</v>
@@ -15115,7 +15106,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>2</v>
       </c>
@@ -15123,13 +15114,13 @@
         <v>1</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>382</v>
+        <v>38</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>43073</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>96</v>
@@ -15138,7 +15129,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>2</v>
       </c>
@@ -15146,13 +15137,13 @@
         <v>1</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>382</v>
+        <v>38</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>43101</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>170</v>
@@ -15161,7 +15152,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>2</v>
       </c>
@@ -15169,13 +15160,13 @@
         <v>1</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>382</v>
+        <v>38</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>43105</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>224</v>
@@ -15184,7 +15175,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>2</v>
       </c>
@@ -15192,13 +15183,13 @@
         <v>1</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>382</v>
+        <v>38</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>43143</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F27" s="0" t="n">
         <v>52</v>
@@ -15207,7 +15198,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>2</v>
       </c>
@@ -15215,13 +15206,13 @@
         <v>1</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>382</v>
+        <v>38</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>43159</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F28" s="0" t="n">
         <v>89</v>
@@ -15230,7 +15221,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>2</v>
       </c>
@@ -15238,13 +15229,13 @@
         <v>1</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>382</v>
+        <v>38</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>43061</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F29" s="0" t="n">
         <v>48</v>
@@ -15253,7 +15244,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>2</v>
       </c>
@@ -15261,13 +15252,13 @@
         <v>1</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>382</v>
+        <v>38</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>43130</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F30" s="0" t="n">
         <v>241</v>
@@ -15290,7 +15281,7 @@
         <v>8048</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F31" s="0" t="n">
         <v>754</v>
@@ -15313,7 +15304,7 @@
         <v>8122</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F32" s="0" t="n">
         <v>2517</v>
@@ -15336,7 +15327,7 @@
         <v>8085</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F33" s="0" t="n">
         <v>1446</v>
@@ -15359,7 +15350,7 @@
         <v>8168</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F34" s="0" t="n">
         <v>507</v>
@@ -15382,7 +15373,7 @@
         <v>8288</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F35" s="0" t="n">
         <v>2557</v>
@@ -15402,10 +15393,10 @@
         <v>47</v>
       </c>
       <c r="D36" s="20" t="s">
+        <v>395</v>
+      </c>
+      <c r="E36" s="0" t="s">
         <v>396</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>397</v>
       </c>
       <c r="F36" s="0" t="n">
         <v>999</v>
@@ -15428,7 +15419,7 @@
         <v>8154</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F37" s="0" t="n">
         <v>935</v>
@@ -15451,7 +15442,7 @@
         <v>8206</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F38" s="0" t="n">
         <v>1009</v>
@@ -15474,7 +15465,7 @@
         <v>8249</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F39" s="0" t="n">
         <v>370</v>
@@ -15497,7 +15488,7 @@
         <v>8304</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F40" s="0" t="n">
         <v>1130</v>
@@ -15520,7 +15511,7 @@
         <v>8058</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F41" s="0" t="n">
         <v>2474</v>
@@ -15543,7 +15534,7 @@
         <v>43002</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F42" s="0" t="n">
         <v>2581</v>
@@ -15566,7 +15557,7 @@
         <v>43030</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F43" s="0" t="n">
         <v>742</v>
@@ -15589,7 +15580,7 @@
         <v>43140</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F44" s="0" t="n">
         <v>3560</v>
@@ -15612,7 +15603,7 @@
         <v>8148</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F45" s="0" t="n">
         <v>4339</v>
@@ -15635,7 +15626,7 @@
         <v>8146</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F46" s="0" t="n">
         <v>2016</v>
@@ -15658,7 +15649,7 @@
         <v>8174</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F47" s="0" t="n">
         <v>555</v>
@@ -15681,7 +15672,7 @@
         <v>8222</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F48" s="0" t="n">
         <v>2503</v>
@@ -15704,7 +15695,7 @@
         <v>8273</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F49" s="0" t="n">
         <v>3241</v>
@@ -15727,7 +15718,7 @@
         <v>8287</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F50" s="0" t="n">
         <v>1457</v>
@@ -15750,7 +15741,7 @@
         <v>43079</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F51" s="0" t="n">
         <v>547</v>
@@ -15773,7 +15764,7 @@
         <v>43090</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F52" s="0" t="n">
         <v>1863</v>
@@ -15796,7 +15787,7 @@
         <v>43135</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F53" s="0" t="n">
         <v>543</v>
@@ -15819,7 +15810,7 @@
         <v>43164</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F54" s="0" t="n">
         <v>496</v>
@@ -15828,7 +15819,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
         <v>2</v>
       </c>
@@ -15836,13 +15827,13 @@
         <v>3</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>382</v>
+        <v>38</v>
       </c>
       <c r="D55" s="0" t="n">
         <v>43029</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F55" s="0" t="n">
         <v>394</v>
@@ -15851,7 +15842,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
         <v>2</v>
       </c>
@@ -15859,13 +15850,13 @@
         <v>3</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>382</v>
+        <v>38</v>
       </c>
       <c r="D56" s="0" t="n">
         <v>43107</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F56" s="0" t="n">
         <v>489</v>
@@ -15874,7 +15865,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
         <v>2</v>
       </c>
@@ -15882,13 +15873,13 @@
         <v>3</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>382</v>
+        <v>38</v>
       </c>
       <c r="D57" s="0" t="n">
         <v>43146</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F57" s="0" t="n">
         <v>44</v>
@@ -15911,7 +15902,7 @@
         <v>43001</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F58" s="0" t="n">
         <v>961</v>
@@ -15934,7 +15925,7 @@
         <v>43036</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F59" s="0" t="n">
         <v>1254</v>
@@ -15957,7 +15948,7 @@
         <v>43120</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F60" s="0" t="n">
         <v>572</v>
@@ -15966,7 +15957,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
         <v>2</v>
       </c>
@@ -15974,13 +15965,13 @@
         <v>3</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>382</v>
+        <v>38</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>43141</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F61" s="0" t="n">
         <v>133</v>
@@ -16003,7 +15994,7 @@
         <v>43059</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F62" s="0" t="n">
         <v>332</v>
@@ -16026,7 +16017,7 @@
         <v>43089</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F63" s="0" t="n">
         <v>419</v>
@@ -16049,7 +16040,7 @@
         <v>43132</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F64" s="0" t="n">
         <v>506</v>
@@ -16058,7 +16049,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
         <v>2</v>
       </c>
@@ -16066,13 +16057,13 @@
         <v>3</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>382</v>
+        <v>38</v>
       </c>
       <c r="D65" s="0" t="n">
         <v>43158</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F65" s="0" t="n">
         <v>88</v>
@@ -16081,7 +16072,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
         <v>2</v>
       </c>
@@ -16089,13 +16080,13 @@
         <v>3</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>382</v>
+        <v>38</v>
       </c>
       <c r="D66" s="0" t="n">
         <v>43168</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F66" s="0" t="n">
         <v>107</v>
@@ -16118,7 +16109,7 @@
         <v>43091</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F67" s="0" t="n">
         <v>173</v>
@@ -16141,7 +16132,7 @@
         <v>43124</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F68" s="0" t="n">
         <v>552</v>
@@ -16150,7 +16141,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
         <v>2</v>
       </c>
@@ -16158,13 +16149,13 @@
         <v>3</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>382</v>
+        <v>38</v>
       </c>
       <c r="D69" s="0" t="n">
         <v>43172</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F69" s="0" t="n">
         <v>453</v>
@@ -16187,7 +16178,7 @@
         <v>43066</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F70" s="0" t="n">
         <v>196</v>
@@ -16210,7 +16201,7 @@
         <v>43080</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F71" s="0" t="n">
         <v>285</v>
@@ -16233,7 +16224,7 @@
         <v>43083</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F72" s="0" t="n">
         <v>189</v>
@@ -16256,7 +16247,7 @@
         <v>43160</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F73" s="0" t="n">
         <v>1882</v>
@@ -16279,7 +16270,7 @@
         <v>43010</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F74" s="0" t="n">
         <v>496</v>
@@ -16302,7 +16293,7 @@
         <v>43034</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F75" s="0" t="n">
         <v>687</v>
@@ -16325,7 +16316,7 @@
         <v>43119</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F76" s="0" t="n">
         <v>1199</v>
@@ -16348,7 +16339,7 @@
         <v>43165</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F77" s="0" t="n">
         <v>711</v>
@@ -16371,7 +16362,7 @@
         <v>43098</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F78" s="0" t="n">
         <v>541</v>
@@ -16394,7 +16385,7 @@
         <v>43134</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F79" s="0" t="n">
         <v>395</v>
@@ -16417,7 +16408,7 @@
         <v>43017</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F80" s="0" t="n">
         <v>126</v>
@@ -16440,7 +16431,7 @@
         <v>43033</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F81" s="0" t="n">
         <v>1102</v>
@@ -16463,7 +16454,7 @@
         <v>43045</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F82" s="0" t="n">
         <v>172</v>
@@ -16486,7 +16477,7 @@
         <v>43118</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F83" s="0" t="n">
         <v>693</v>
@@ -16509,7 +16500,7 @@
         <v>43127</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="F84" s="0" t="n">
         <v>1279</v>
@@ -16532,7 +16523,7 @@
         <v>43167</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F85" s="0" t="n">
         <v>594</v>
@@ -16555,7 +16546,7 @@
         <v>43007</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F86" s="0" t="n">
         <v>924</v>
@@ -16578,7 +16569,7 @@
         <v>43009</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F87" s="0" t="n">
         <v>1928</v>
@@ -16601,7 +16592,7 @@
         <v>43053</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F88" s="0" t="n">
         <v>232</v>
@@ -16624,7 +16615,7 @@
         <v>43081</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F89" s="0" t="n">
         <v>859</v>
@@ -16647,7 +16638,7 @@
         <v>43128</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="F90" s="0" t="n">
         <v>1198</v>
@@ -16670,7 +16661,7 @@
         <v>43015</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F91" s="0" t="n">
         <v>122</v>
@@ -16693,7 +16684,7 @@
         <v>43039</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F92" s="0" t="n">
         <v>121</v>
@@ -16716,7 +16707,7 @@
         <v>43057</v>
       </c>
       <c r="E93" s="0" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F93" s="0" t="n">
         <v>39</v>
@@ -16739,7 +16730,7 @@
         <v>43169</v>
       </c>
       <c r="E94" s="0" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="F94" s="0" t="n">
         <v>540</v>
@@ -16762,7 +16753,7 @@
         <v>43003</v>
       </c>
       <c r="E95" s="0" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F95" s="0" t="n">
         <v>528</v>
@@ -16785,7 +16776,7 @@
         <v>43011</v>
       </c>
       <c r="E96" s="0" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F96" s="0" t="n">
         <v>1334</v>
@@ -16808,7 +16799,7 @@
         <v>43103</v>
       </c>
       <c r="E97" s="0" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F97" s="0" t="n">
         <v>1292</v>
@@ -16831,7 +16822,7 @@
         <v>43109</v>
       </c>
       <c r="E98" s="0" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F98" s="0" t="n">
         <v>4052</v>
@@ -16854,7 +16845,7 @@
         <v>43166</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F99" s="0" t="n">
         <v>2398</v>
@@ -16877,7 +16868,7 @@
         <v>43097</v>
       </c>
       <c r="E100" s="0" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F100" s="0" t="n">
         <v>636</v>
@@ -16900,7 +16891,7 @@
         <v>43126</v>
       </c>
       <c r="E101" s="0" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F101" s="0" t="n">
         <v>1752</v>
@@ -16923,7 +16914,7 @@
         <v>43043</v>
       </c>
       <c r="E102" s="0" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F102" s="0" t="n">
         <v>4921</v>
@@ -16946,7 +16937,7 @@
         <v>43144</v>
       </c>
       <c r="E103" s="0" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F103" s="0" t="n">
         <v>1765</v>
@@ -16969,7 +16960,7 @@
         <v>43122</v>
       </c>
       <c r="E104" s="0" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F104" s="0" t="n">
         <v>152</v>
@@ -17002,8 +16993,8 @@
   </sheetPr>
   <dimension ref="A1:G105"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A84" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I11" activeCellId="1" sqref="C22:C25 I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17054,7 +17045,7 @@
         <v>17038</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>535</v>
@@ -17077,7 +17068,7 @@
         <v>17090</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>731</v>
@@ -17100,7 +17091,7 @@
         <v>17157</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>162</v>
@@ -17123,7 +17114,7 @@
         <v>17101</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>825</v>
@@ -17146,7 +17137,7 @@
         <v>17159</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>839</v>
@@ -17166,10 +17157,10 @@
         <v>209</v>
       </c>
       <c r="D7" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>471</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>472</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>780</v>
@@ -17192,7 +17183,7 @@
         <v>17172</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>679</v>
@@ -17215,7 +17206,7 @@
         <v>17028</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>388</v>
@@ -17238,7 +17229,7 @@
         <v>17116</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>423</v>
@@ -17261,7 +17252,7 @@
         <v>17194</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>96</v>
@@ -17278,13 +17269,13 @@
         <v>4</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>17174</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>239</v>
@@ -17307,7 +17298,7 @@
         <v>17105</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>341</v>
@@ -17330,7 +17321,7 @@
         <v>17183</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>363</v>
@@ -17353,7 +17344,7 @@
         <v>17040</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>750</v>
@@ -17370,13 +17361,13 @@
         <v>4</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>17035</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>715</v>
@@ -17399,7 +17390,7 @@
         <v>17121</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>327</v>
@@ -17422,7 +17413,7 @@
         <v>17144</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>271</v>
@@ -17445,7 +17436,7 @@
         <v>17209</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>926</v>
@@ -17468,7 +17459,7 @@
         <v>17901</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>1338</v>
@@ -17491,7 +17482,7 @@
         <v>17902</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>1765</v>
@@ -17514,7 +17505,7 @@
         <v>17126</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>415</v>
@@ -17537,7 +17528,7 @@
         <v>17130</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>438</v>
@@ -17560,7 +17551,7 @@
         <v>17153</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>300</v>
@@ -17583,7 +17574,7 @@
         <v>17087</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>334</v>
@@ -17606,7 +17597,7 @@
         <v>17097</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>302</v>
@@ -17629,7 +17620,7 @@
         <v>17173</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F27" s="0" t="n">
         <v>261</v>
@@ -17652,7 +17643,7 @@
         <v>17057</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F28" s="0" t="n">
         <v>1268</v>
@@ -17675,7 +17666,7 @@
         <v>17068</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="F29" s="0" t="n">
         <v>288</v>
@@ -17698,7 +17689,7 @@
         <v>17070</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F30" s="0" t="n">
         <v>163</v>
@@ -17721,7 +17712,7 @@
         <v>17081</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F31" s="0" t="n">
         <v>439</v>
@@ -17744,7 +17735,7 @@
         <v>17191</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F32" s="0" t="n">
         <v>233</v>
@@ -17767,7 +17758,7 @@
         <v>17204</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F33" s="0" t="n">
         <v>1195</v>
@@ -17790,7 +17781,7 @@
         <v>17055</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F34" s="0" t="n">
         <v>204</v>
@@ -17813,7 +17804,7 @@
         <v>17076</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F35" s="0" t="n">
         <v>177</v>
@@ -17836,7 +17827,7 @@
         <v>17195</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F36" s="0" t="n">
         <v>480</v>
@@ -17859,7 +17850,7 @@
         <v>17232</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F37" s="0" t="n">
         <v>223</v>
@@ -17882,7 +17873,7 @@
         <v>17050</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F38" s="0" t="n">
         <v>999</v>
@@ -17899,13 +17890,13 @@
         <v>4</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>17123</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F39" s="0" t="n">
         <v>457</v>
@@ -17928,7 +17919,7 @@
         <v>17210</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F40" s="0" t="n">
         <v>911</v>
@@ -17951,7 +17942,7 @@
         <v>17217</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F41" s="0" t="n">
         <v>479</v>
@@ -17974,7 +17965,7 @@
         <v>17004</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F42" s="0" t="n">
         <v>797</v>
@@ -17997,7 +17988,7 @@
         <v>17018</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F43" s="0" t="n">
         <v>713</v>
@@ -18020,7 +18011,7 @@
         <v>17175</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F44" s="0" t="n">
         <v>808</v>
@@ -18043,7 +18034,7 @@
         <v>17198</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F45" s="0" t="n">
         <v>741</v>
@@ -18066,7 +18057,7 @@
         <v>17222</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F46" s="0" t="n">
         <v>162</v>
@@ -18089,7 +18080,7 @@
         <v>17225</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F47" s="0" t="n">
         <v>386</v>
@@ -18106,13 +18097,13 @@
         <v>4</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D48" s="0" t="n">
         <v>17218</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F48" s="0" t="n">
         <v>840</v>
@@ -18135,7 +18126,7 @@
         <v>17098</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F49" s="0" t="n">
         <v>462</v>
@@ -18158,7 +18149,7 @@
         <v>17162</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F50" s="0" t="n">
         <v>256</v>
@@ -18175,13 +18166,13 @@
         <v>4</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D51" s="0" t="n">
         <v>17058</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F51" s="0" t="n">
         <v>276</v>
@@ -18198,13 +18189,13 @@
         <v>4</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D52" s="0" t="n">
         <v>17065</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F52" s="0" t="n">
         <v>489</v>
@@ -18221,13 +18212,13 @@
         <v>4</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D53" s="0" t="n">
         <v>17071</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F53" s="0" t="n">
         <v>1466</v>
@@ -18250,7 +18241,7 @@
         <v>17010</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F54" s="0" t="n">
         <v>439</v>
@@ -18273,7 +18264,7 @@
         <v>17149</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F55" s="0" t="n">
         <v>511</v>
@@ -18296,7 +18287,7 @@
         <v>17165</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F56" s="0" t="n">
         <v>842</v>
@@ -18319,7 +18310,7 @@
         <v>17208</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F57" s="0" t="n">
         <v>1345</v>
@@ -18342,7 +18333,7 @@
         <v>17003</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F58" s="0" t="n">
         <v>180</v>
@@ -18365,7 +18356,7 @@
         <v>17109</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="F59" s="0" t="n">
         <v>958</v>
@@ -18388,7 +18379,7 @@
         <v>17154</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="F60" s="0" t="n">
         <v>169</v>
@@ -18411,7 +18402,7 @@
         <v>17200</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F61" s="0" t="n">
         <v>823</v>
@@ -18434,7 +18425,7 @@
         <v>17026</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F62" s="0" t="n">
         <v>776</v>
@@ -18457,7 +18448,7 @@
         <v>17052</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="F63" s="0" t="n">
         <v>178</v>
@@ -18480,7 +18471,7 @@
         <v>17075</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F64" s="0" t="n">
         <v>458</v>
@@ -18503,7 +18494,7 @@
         <v>17111</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="F65" s="0" t="n">
         <v>1465</v>
@@ -18523,10 +18514,10 @@
         <v>126</v>
       </c>
       <c r="D66" s="0" t="s">
+        <v>531</v>
+      </c>
+      <c r="E66" s="0" t="s">
         <v>532</v>
-      </c>
-      <c r="E66" s="0" t="s">
-        <v>533</v>
       </c>
       <c r="F66" s="0" t="n">
         <v>625</v>
@@ -18549,7 +18540,7 @@
         <v>17074</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="F67" s="0" t="n">
         <v>778</v>
@@ -18572,7 +18563,7 @@
         <v>17151</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="F68" s="0" t="n">
         <v>244</v>
@@ -18595,7 +18586,7 @@
         <v>17182</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="F69" s="0" t="n">
         <v>379</v>
@@ -18618,7 +18609,7 @@
         <v>17230</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F70" s="0" t="n">
         <v>785</v>
@@ -18641,7 +18632,7 @@
         <v>17030</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F71" s="0" t="n">
         <v>949</v>
@@ -18664,7 +18655,7 @@
         <v>17128</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F72" s="0" t="n">
         <v>579</v>
@@ -18687,7 +18678,7 @@
         <v>17129</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="F73" s="0" t="n">
         <v>181</v>
@@ -18710,7 +18701,7 @@
         <v>17188</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="F74" s="0" t="n">
         <v>220</v>
@@ -18733,7 +18724,7 @@
         <v>17012</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F75" s="0" t="n">
         <v>1676</v>
@@ -18756,7 +18747,7 @@
         <v>17031</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="F76" s="0" t="n">
         <v>279</v>
@@ -18779,7 +18770,7 @@
         <v>17088</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F77" s="0" t="n">
         <v>827</v>
@@ -18802,7 +18793,7 @@
         <v>17228</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F78" s="0" t="n">
         <v>401</v>
@@ -18825,7 +18816,7 @@
         <v>17029</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="F79" s="0" t="n">
         <v>258</v>
@@ -18848,7 +18839,7 @@
         <v>17051</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F80" s="0" t="n">
         <v>307</v>
@@ -18871,7 +18862,7 @@
         <v>17171</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F81" s="0" t="n">
         <v>267</v>
@@ -18894,7 +18885,7 @@
         <v>17196</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F82" s="0" t="n">
         <v>345</v>
@@ -18917,7 +18908,7 @@
         <v>17100</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F83" s="0" t="n">
         <v>294</v>
@@ -18940,7 +18931,7 @@
         <v>17106</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F84" s="0" t="n">
         <v>202</v>
@@ -18963,7 +18954,7 @@
         <v>17042</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="F85" s="0" t="n">
         <v>672</v>
@@ -18986,7 +18977,7 @@
         <v>17135</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="F86" s="0" t="n">
         <v>542</v>
@@ -19009,7 +19000,7 @@
         <v>17064</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="F87" s="0" t="n">
         <v>408</v>
@@ -19032,7 +19023,7 @@
         <v>17143</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F88" s="0" t="n">
         <v>210</v>
@@ -19055,7 +19046,7 @@
         <v>17227</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F89" s="0" t="n">
         <v>204</v>
@@ -19078,7 +19069,7 @@
         <v>17014</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F90" s="0" t="n">
         <v>87</v>
@@ -19101,7 +19092,7 @@
         <v>17041</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F91" s="0" t="n">
         <v>330</v>
@@ -19124,7 +19115,7 @@
         <v>17115</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="F92" s="0" t="n">
         <v>373</v>
@@ -19147,7 +19138,7 @@
         <v>17119</v>
       </c>
       <c r="E93" s="0" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F93" s="0" t="n">
         <v>115</v>
@@ -19170,7 +19161,7 @@
         <v>17136</v>
       </c>
       <c r="E94" s="0" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F94" s="0" t="n">
         <v>274</v>
@@ -19193,7 +19184,7 @@
         <v>17221</v>
       </c>
       <c r="E95" s="0" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F95" s="0" t="n">
         <v>5562</v>
@@ -19216,7 +19207,7 @@
         <v>17226</v>
       </c>
       <c r="E96" s="0" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="F96" s="0" t="n">
         <v>1166</v>
@@ -19239,7 +19230,7 @@
         <v>17234</v>
       </c>
       <c r="E97" s="0" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F97" s="0" t="n">
         <v>249</v>
@@ -19262,7 +19253,7 @@
         <v>17021</v>
       </c>
       <c r="E98" s="0" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F98" s="0" t="n">
         <v>202</v>
@@ -19285,7 +19276,7 @@
         <v>17085</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F99" s="0" t="n">
         <v>386</v>
@@ -19308,7 +19299,7 @@
         <v>17197</v>
       </c>
       <c r="E100" s="0" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F100" s="0" t="n">
         <v>166</v>
@@ -19331,7 +19322,7 @@
         <v>17203</v>
       </c>
       <c r="E101" s="0" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F101" s="0" t="n">
         <v>224</v>
@@ -19354,7 +19345,7 @@
         <v>17205</v>
       </c>
       <c r="E102" s="0" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F102" s="0" t="n">
         <v>250</v>
@@ -19377,7 +19368,7 @@
         <v>17168</v>
       </c>
       <c r="E103" s="0" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F103" s="0" t="n">
         <v>515</v>
@@ -19400,7 +19391,7 @@
         <v>17216</v>
       </c>
       <c r="E104" s="0" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="F104" s="0" t="n">
         <v>216</v>
@@ -19423,7 +19414,7 @@
         <v>8082</v>
       </c>
       <c r="E105" s="0" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="F105" s="0" t="n">
         <v>1564</v>
@@ -19452,8 +19443,8 @@
   </sheetPr>
   <dimension ref="A1:G105"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A90" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19504,7 +19495,7 @@
         <v>8242</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>282</v>
@@ -19521,13 +19512,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>8066</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>2096</v>
@@ -19544,13 +19535,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>8069</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>4726</v>
@@ -19567,13 +19558,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>578</v>
+        <v>248</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>8179</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>915</v>
@@ -19582,7 +19573,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
@@ -19590,13 +19581,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>578</v>
+        <v>248</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>8290</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>2139</v>
@@ -19619,7 +19610,7 @@
         <v>8153</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>793</v>
@@ -19636,13 +19627,13 @@
         <v>1</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>582</v>
+        <v>253</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>8256</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>889</v>
@@ -19651,7 +19642,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>5</v>
       </c>
@@ -19659,13 +19650,13 @@
         <v>1</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>582</v>
+        <v>253</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>8294</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>3144</v>
@@ -19674,7 +19665,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>5</v>
       </c>
@@ -19682,13 +19673,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>582</v>
+        <v>253</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>8306</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>748</v>
@@ -19697,7 +19688,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>5</v>
       </c>
@@ -19705,13 +19696,13 @@
         <v>1</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>582</v>
+        <v>253</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>8039</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>557</v>
@@ -19720,7 +19711,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>5</v>
       </c>
@@ -19728,13 +19719,13 @@
         <v>1</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>582</v>
+        <v>253</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>8042</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>3289</v>
@@ -19743,7 +19734,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>5</v>
       </c>
@@ -19751,13 +19742,13 @@
         <v>1</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>582</v>
+        <v>253</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>8081</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>493</v>
@@ -19766,7 +19757,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>5</v>
       </c>
@@ -19774,13 +19765,13 @@
         <v>1</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>582</v>
+        <v>253</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>8097</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>1610</v>
@@ -19789,7 +19780,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>5</v>
       </c>
@@ -19797,13 +19788,13 @@
         <v>1</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>582</v>
+        <v>253</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>8234</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>4815</v>
@@ -19826,7 +19817,7 @@
         <v>8059</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>460</v>
@@ -19849,7 +19840,7 @@
         <v>8061</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>2236</v>
@@ -19872,7 +19863,7 @@
         <v>8139</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>232</v>
@@ -19895,7 +19886,7 @@
         <v>8277</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>219</v>
@@ -19904,7 +19895,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>5</v>
       </c>
@@ -19912,13 +19903,13 @@
         <v>1</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>578</v>
+        <v>248</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>8223</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>2524</v>
@@ -19927,7 +19918,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>5</v>
       </c>
@@ -19935,13 +19926,13 @@
         <v>1</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>578</v>
+        <v>248</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>8087</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>186</v>
@@ -19950,7 +19941,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>5</v>
       </c>
@@ -19958,13 +19949,13 @@
         <v>1</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>582</v>
+        <v>253</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>8276</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>340</v>
@@ -19973,7 +19964,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>5</v>
       </c>
@@ -19981,13 +19972,13 @@
         <v>1</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>582</v>
+        <v>253</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>8134</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>1108</v>
@@ -19996,7 +19987,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>5</v>
       </c>
@@ -20004,13 +19995,13 @@
         <v>1</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>582</v>
+        <v>253</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>8137</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>370</v>
@@ -20019,7 +20010,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>5</v>
       </c>
@@ -20027,13 +20018,13 @@
         <v>1</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>582</v>
+        <v>253</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>8207</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>3043</v>
@@ -20056,7 +20047,7 @@
         <v>8002</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>287</v>
@@ -20079,7 +20070,7 @@
         <v>8084</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="F27" s="0" t="n">
         <v>1546</v>
@@ -20102,7 +20093,7 @@
         <v>8178</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="F28" s="0" t="n">
         <v>545</v>
@@ -20125,7 +20116,7 @@
         <v>8062</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="F29" s="0" t="n">
         <v>1431</v>
@@ -20148,7 +20139,7 @@
         <v>8229</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="F30" s="0" t="n">
         <v>628</v>
@@ -20171,7 +20162,7 @@
         <v>8095</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="F31" s="0" t="n">
         <v>80</v>
@@ -20194,7 +20185,7 @@
         <v>8128</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="F32" s="0" t="n">
         <v>742</v>
@@ -20217,7 +20208,7 @@
         <v>8239</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="F33" s="0" t="n">
         <v>672</v>
@@ -20240,7 +20231,7 @@
         <v>8034</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="F34" s="0" t="n">
         <v>1101</v>
@@ -20263,7 +20254,7 @@
         <v>8055</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="F35" s="0" t="n">
         <v>778</v>
@@ -20286,7 +20277,7 @@
         <v>8070</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="F36" s="0" t="n">
         <v>398</v>
@@ -20309,7 +20300,7 @@
         <v>8079</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="F37" s="0" t="n">
         <v>391</v>
@@ -20332,7 +20323,7 @@
         <v>8212</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="F38" s="0" t="n">
         <v>611</v>
@@ -20355,7 +20346,7 @@
         <v>8308</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="F39" s="0" t="n">
         <v>166</v>
@@ -20378,7 +20369,7 @@
         <v>8188</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="F40" s="0" t="n">
         <v>157</v>
@@ -20401,7 +20392,7 @@
         <v>8255</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="F41" s="0" t="n">
         <v>184</v>
@@ -20424,7 +20415,7 @@
         <v>8149</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="F42" s="0" t="n">
         <v>1206</v>
@@ -20447,7 +20438,7 @@
         <v>8151</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="F43" s="0" t="n">
         <v>573</v>
@@ -20470,7 +20461,7 @@
         <v>8225</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="F44" s="0" t="n">
         <v>119</v>
@@ -20493,7 +20484,7 @@
         <v>8271</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="F45" s="0" t="n">
         <v>83</v>
@@ -20516,7 +20507,7 @@
         <v>8144</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="F46" s="0" t="n">
         <v>876</v>
@@ -20539,7 +20530,7 @@
         <v>8109</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="F47" s="0" t="n">
         <v>279</v>
@@ -20562,7 +20553,7 @@
         <v>8160</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="F48" s="0" t="n">
         <v>418</v>
@@ -20585,7 +20576,7 @@
         <v>8004</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="F49" s="0" t="n">
         <v>281</v>
@@ -20608,7 +20599,7 @@
         <v>8111</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="F50" s="0" t="n">
         <v>272</v>
@@ -20631,7 +20622,7 @@
         <v>8129</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="F51" s="0" t="n">
         <v>700</v>
@@ -20651,10 +20642,10 @@
         <v>294</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="F52" s="0" t="n">
         <v>2254</v>
@@ -20677,7 +20668,7 @@
         <v>8246</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="F53" s="0" t="n">
         <v>2256</v>
@@ -20700,7 +20691,7 @@
         <v>8247</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="F54" s="0" t="n">
         <v>1401</v>
@@ -20723,7 +20714,7 @@
         <v>8303</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="F55" s="0" t="n">
         <v>320</v>
@@ -20746,7 +20737,7 @@
         <v>8224</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="F56" s="0" t="n">
         <v>1232</v>
@@ -20769,7 +20760,7 @@
         <v>8100</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="F57" s="0" t="n">
         <v>2702</v>
@@ -20792,7 +20783,7 @@
         <v>8116</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="F58" s="0" t="n">
         <v>733</v>
@@ -20815,7 +20806,7 @@
         <v>8243</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="F59" s="0" t="n">
         <v>185</v>
@@ -20838,7 +20829,7 @@
         <v>8280</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="F60" s="0" t="n">
         <v>116</v>
@@ -20861,7 +20852,7 @@
         <v>8901</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="F61" s="0" t="n">
         <v>279</v>
@@ -20884,7 +20875,7 @@
         <v>8199</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="F62" s="0" t="n">
         <v>924</v>
@@ -20907,7 +20898,7 @@
         <v>8117</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="F63" s="0" t="n">
         <v>3133</v>
@@ -20930,7 +20921,7 @@
         <v>8150</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="F64" s="0" t="n">
         <v>347</v>
@@ -20953,7 +20944,7 @@
         <v>8201</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="F65" s="0" t="n">
         <v>575</v>
@@ -20976,7 +20967,7 @@
         <v>8253</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="F66" s="0" t="n">
         <v>159</v>
@@ -20999,7 +20990,7 @@
         <v>8265</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="F67" s="0" t="n">
         <v>2077</v>
@@ -21022,7 +21013,7 @@
         <v>8272</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="F68" s="0" t="n">
         <v>219</v>
@@ -21042,10 +21033,10 @@
         <v>294</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="F69" s="0" t="n">
         <v>181</v>
@@ -21068,7 +21059,7 @@
         <v>8131</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="F70" s="0" t="n">
         <v>1059</v>
@@ -21091,7 +21082,7 @@
         <v>8195</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="F71" s="0" t="n">
         <v>100</v>
@@ -21114,7 +21105,7 @@
         <v>8275</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="F72" s="0" t="n">
         <v>329</v>
@@ -21137,7 +21128,7 @@
         <v>8241</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="F73" s="0" t="n">
         <v>90</v>
@@ -21160,7 +21151,7 @@
         <v>17063</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="F74" s="0" t="n">
         <v>248</v>
@@ -21180,10 +21171,10 @@
         <v>294</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="F75" s="0" t="n">
         <v>278</v>
@@ -21206,7 +21197,7 @@
         <v>8078</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="F76" s="0" t="n">
         <v>265</v>
@@ -21229,7 +21220,7 @@
         <v>8130</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="F77" s="0" t="n">
         <v>136</v>
@@ -21252,7 +21243,7 @@
         <v>8045</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="F78" s="0" t="n">
         <v>89</v>
@@ -21275,7 +21266,7 @@
         <v>8050</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="F79" s="0" t="n">
         <v>175</v>
@@ -21298,7 +21289,7 @@
         <v>8080</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="F80" s="0" t="n">
         <v>45</v>
@@ -21321,7 +21312,7 @@
         <v>8142</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="F81" s="0" t="n">
         <v>179</v>
@@ -21344,7 +21335,7 @@
         <v>8177</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="F82" s="0" t="n">
         <v>47</v>
@@ -21367,7 +21358,7 @@
         <v>8299</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="F83" s="0" t="n">
         <v>439</v>
@@ -21390,7 +21381,7 @@
         <v>17096</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="F84" s="0" t="n">
         <v>205</v>
@@ -21413,7 +21404,7 @@
         <v>17170</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="F85" s="0" t="n">
         <v>222</v>
@@ -21433,10 +21424,10 @@
         <v>273</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="F86" s="0" t="n">
         <v>448</v>
@@ -21459,7 +21450,7 @@
         <v>8057</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="F87" s="0" t="n">
         <v>69</v>
@@ -21482,7 +21473,7 @@
         <v>8216</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="F88" s="0" t="n">
         <v>31</v>
@@ -21505,7 +21496,7 @@
         <v>8293</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="F89" s="0" t="n">
         <v>268</v>
@@ -21528,7 +21519,7 @@
         <v>8903</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="F90" s="0" t="n">
         <v>241</v>
@@ -21551,7 +21542,7 @@
         <v>8093</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="F91" s="0" t="n">
         <v>28</v>
@@ -21574,7 +21565,7 @@
         <v>8190</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="F92" s="0" t="n">
         <v>298</v>
@@ -21597,7 +21588,7 @@
         <v>25100</v>
       </c>
       <c r="E93" s="0" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="F93" s="0" t="n">
         <v>233</v>
@@ -21620,7 +21611,7 @@
         <v>8052</v>
       </c>
       <c r="E94" s="0" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="F94" s="0" t="n">
         <v>176</v>
@@ -21643,7 +21634,7 @@
         <v>17037</v>
       </c>
       <c r="E95" s="0" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="F95" s="0" t="n">
         <v>162</v>
@@ -21666,7 +21657,7 @@
         <v>17080</v>
       </c>
       <c r="E96" s="0" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="F96" s="0" t="n">
         <v>200</v>
@@ -21689,7 +21680,7 @@
         <v>17134</v>
       </c>
       <c r="E97" s="0" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="F97" s="0" t="n">
         <v>307</v>
@@ -21712,7 +21703,7 @@
         <v>17201</v>
       </c>
       <c r="E98" s="0" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="F98" s="0" t="n">
         <v>185</v>
@@ -21735,7 +21726,7 @@
         <v>17192</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="F99" s="0" t="n">
         <v>200</v>
@@ -21758,7 +21749,7 @@
         <v>17091</v>
       </c>
       <c r="E100" s="0" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="F100" s="0" t="n">
         <v>533</v>
@@ -21781,7 +21772,7 @@
         <v>17107</v>
       </c>
       <c r="E101" s="0" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="F101" s="0" t="n">
         <v>365</v>
@@ -21804,7 +21795,7 @@
         <v>17112</v>
       </c>
       <c r="E102" s="0" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="F102" s="0" t="n">
         <v>222</v>
@@ -21827,7 +21818,7 @@
         <v>17224</v>
       </c>
       <c r="E103" s="0" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="F103" s="0" t="n">
         <v>410</v>
@@ -21850,7 +21841,7 @@
         <v>17125</v>
       </c>
       <c r="E104" s="0" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="F104" s="0" t="n">
         <v>165</v>
@@ -21873,7 +21864,7 @@
         <v>17043</v>
       </c>
       <c r="E105" s="0" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="F105" s="0" t="n">
         <v>191</v>

</xml_diff>